<commit_message>
Add `task-2` in `financial-mathematics`
</commit_message>
<xml_diff>
--- a/3-course-6-semester/game-theory/Бронников ПМ-1901 - Антагон 2x2.xlsx
+++ b/3-course-6-semester/game-theory/Бронников ПМ-1901 - Антагон 2x2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\egor\github\university\3-course-6-semester\game-theory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567E2C47-ADDC-41CE-A412-531AE958ACC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A4AA022-B430-46DB-BB53-ED7BEDD316F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A595A620-D18C-44B8-8488-DC903CB40E6E}"/>
   </bookViews>
@@ -2780,7 +2780,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2821,6 +2821,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="18">
+        <f>IF((E8-E7)/(D7-E7-D8+E8)&lt;0,1,(E8-E7)/(D7-E7-D8+E8))</f>
         <v>0.5</v>
       </c>
       <c r="E6" s="19">
@@ -2840,6 +2841,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="15">
+        <f>IF((E8-D8)/(D7-E7-D8+E8)&lt;0,1,(E8-D8)/(D7-E7-D8+E8))</f>
         <v>0.25</v>
       </c>
       <c r="D7" s="2">

</xml_diff>